<commit_message>
to check the verion v1.1
</commit_message>
<xml_diff>
--- a/SFF_testscenarios.xlsx
+++ b/SFF_testscenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coeus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eDrive data\Git Repositories\new-folder-by-sana\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
   <si>
     <t>Scope of Prototype 1</t>
   </si>
@@ -219,13 +219,16 @@
   </si>
   <si>
     <t>system will save the form and will redirect to dashboard with a success message</t>
+  </si>
+  <si>
+    <t>2nd line to check the versions history</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +253,13 @@
       <sz val="12.1"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -278,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -301,11 +311,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -333,6 +380,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,9 +670,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -662,40 +720,34 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="31.5" thickBot="1">
+    <row r="4" spans="1:5" ht="25.5" customHeight="1" thickBot="1">
+      <c r="A4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1">
       <c r="A5" s="3"/>
       <c r="B5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="31.5" thickBot="1">
       <c r="A6" s="3"/>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -710,7 +762,7 @@
     <row r="7" spans="1:5" ht="31.5" thickBot="1">
       <c r="A7" s="3"/>
       <c r="B7" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -725,48 +777,48 @@
     <row r="8" spans="1:5" ht="31.5" thickBot="1">
       <c r="A8" s="3"/>
       <c r="B8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" thickBot="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="16.5" thickBot="1">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="16.5" thickBot="1">
       <c r="A11" s="3"/>
       <c r="B11" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>9</v>
@@ -775,28 +827,28 @@
     <row r="12" spans="1:5" ht="16.5" thickBot="1">
       <c r="A12" s="3"/>
       <c r="B12" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" thickBot="1">
       <c r="A13" s="3"/>
       <c r="B13" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>12</v>
@@ -805,24 +857,32 @@
     <row r="14" spans="1:5" ht="16.5" thickBot="1">
       <c r="A14" s="3"/>
       <c r="B14" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1">
+    <row r="15" spans="1:5" ht="16.5" thickBot="1">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1">
       <c r="A16" s="3"/>
@@ -831,76 +891,68 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" ht="16.5" thickBot="1">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1">
       <c r="A17" s="3"/>
-      <c r="B17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="31.5" thickBot="1">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" thickBot="1">
       <c r="A18" s="3"/>
       <c r="B18" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="31.5" thickBot="1">
       <c r="A19" s="3"/>
       <c r="B19" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16.5" thickBot="1">
+    <row r="20" spans="1:5" ht="31.5" thickBot="1">
       <c r="A20" s="3"/>
       <c r="B20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="C21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="46.5" thickBot="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>9</v>
@@ -909,110 +961,110 @@
     <row r="22" spans="1:5" ht="46.5" thickBot="1">
       <c r="A22" s="3"/>
       <c r="B22" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="46.5" thickBot="1">
+      <c r="A23" s="3"/>
+      <c r="B23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="31.5" thickBot="1">
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="3"/>
-      <c r="B24" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="27" thickBot="1">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="31.5" thickBot="1">
       <c r="A25" s="3"/>
       <c r="B25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="27" thickBot="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="61.5" thickBot="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="E26" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="27" thickBot="1">
+    <row r="27" spans="1:5" ht="61.5" thickBot="1">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>45</v>
+      <c r="D27" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1">
+    <row r="28" spans="1:5" ht="27" thickBot="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="27" thickBot="1">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>9</v>
@@ -1021,22 +1073,22 @@
     <row r="30" spans="1:5" ht="27" thickBot="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="39.75" thickBot="1">
+    <row r="31" spans="1:5" ht="27" thickBot="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>7</v>
@@ -1048,118 +1100,136 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1">
+    <row r="32" spans="1:5" ht="39.75" thickBot="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="27" thickBot="1">
+    <row r="33" spans="1:5" ht="15.75" thickBot="1">
       <c r="A33" s="3"/>
       <c r="B33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="27" thickBot="1">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="C34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5" ht="27" thickBot="1">
+    <row r="35" spans="1:5" ht="15.75" thickBot="1">
       <c r="A35" s="3"/>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" ht="27" thickBot="1">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="3" t="s">
+      <c r="C36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="7" t="s">
+    <row r="37" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A37" s="3"/>
+      <c r="B37" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="3" t="s">
+      <c r="C37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:5" ht="16.5" thickBot="1">
+      <c r="E37" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1">
       <c r="A38" s="3"/>
-      <c r="B38" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="27" thickBot="1">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" ht="16.5" thickBot="1">
       <c r="A39" s="3"/>
       <c r="B39" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="27" thickBot="1">
+      <c r="A40" s="3"/>
+      <c r="B40" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="3" t="s">
+      <c r="C40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:E4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
This is the version v1.3 of test scenarios (SFF)
</commit_message>
<xml_diff>
--- a/SFF_testscenarios.xlsx
+++ b/SFF_testscenarios.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Prototype1" sheetId="1" r:id="rId1"/>
+    <sheet name="Prototype2" sheetId="2" r:id="rId2"/>
+    <sheet name="Alpha Sprint 3 Analytics" sheetId="3" r:id="rId3"/>
+    <sheet name="Alpha Sprint 3 AB testing" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -23,8 +26,236 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>coeus</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>coeus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Login Screen.
+Create form Screen
+Editor Should have following options in edit text area i.e.
+Short text.
+Long text
+Multiple choice.
+Drop down.
+Yes / No
+Legal text.
+Thank you text.
+Error texts for each of the fields above.
+Compulsory or optionals texts.
+Listing Page.
+Ability to upload logos
+Integration of Preview functionality.
+Template functionality:Only use form template(no fromt scratch)
+Customer satisfaction survey with predefined fields
+Have preview functionality.
+Have use this template button.
+DB design and architecture .</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>coeus</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>coeus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Save all form submissions in a database.
+Ability to adjust form UI .This will include i.e.
+Set color schemes
+Set font types
+Every form Should Have at identifier (id form).
+Resultant form should responsive .
+Add “Powered by eKomi” under every form .
+If the form is too long, auto display a scroll.
+Define ability to set a call back function in the form.
+Ability to mark a form as default .
+Define an HTTP API to display the form.
+Add auto-submission from smart form to default eKomi forms.
+Integration with eApps Appstore.
+Hosting on Amazon webservices, add sub domain</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>coeus</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>coeus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Each CSV has following value:
+form_id
+transaction id
+shop id
+total dropout : total number of dropped form for a specific transaction id (tid) of a form.
+unique dropout : if form is not complete in a single attempt then that is 1, otherwise 0.
+last filled field : for each dropout their is last filled field, we save last dropout one.
+total time spent : add all time spent on all forms(total dropout time + form complete time)
+form complete: if form submit, then 1 otherwise 0
+database user name: sff
+password: b5vlpt9602b
+URL: http://sff.coeus-solutions.de/phpmyadmin
+Show less</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>coeus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+.i.e time out will consider when user will close the form</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>coeus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+System will show a message "you have already submitted this form"</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>coeus</author>
+  </authors>
+  <commentList>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>coeus:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Analytics within the specified duration will be considered only</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="167">
   <si>
     <t>Scope of Prototype 1</t>
   </si>
@@ -221,14 +452,317 @@
     <t>system will save the form and will redirect to dashboard with a success message</t>
   </si>
   <si>
-    <t>2nd line to check the versions history</t>
+    <t>Scope of Prototype 2</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Click at "make as default" link against any survey on dashboard listing</t>
+  </si>
+  <si>
+    <t>System will open a popup and prompt the user for confirmation</t>
+  </si>
+  <si>
+    <t>that survey wil be saved as default survey and system will show a success message</t>
+  </si>
+  <si>
+    <t>that popup will be closed without any furhter action</t>
+  </si>
+  <si>
+    <t>click at "Use this template" button without selecting any predefined template</t>
+  </si>
+  <si>
+    <t>click at "Use this template" button after selecting any predefined template</t>
+  </si>
+  <si>
+    <t>there will be three panels (left panel for drag/drop elements , right panel with predefined elements of selected template and a thankyou panel) and two buttons (upload logo and adjust form UI)</t>
+  </si>
+  <si>
+    <t>Click at "Adjust formUI" button</t>
+  </si>
+  <si>
+    <t>system will open a popup with three options .i.e form text style , form text color and form background color</t>
+  </si>
+  <si>
+    <t>Select color for text and background from the color picker , and select text style from dropdown and click at "save" button</t>
+  </si>
+  <si>
+    <t>system will save the changes and will apply to that specific survey</t>
+  </si>
+  <si>
+    <t>system will save the form and will redirect to distribution page with a success message</t>
+  </si>
+  <si>
+    <t>After successfuly saving the form the user will be on survey distribution page</t>
+  </si>
+  <si>
+    <t>there system will show a link which user can send to others for the survey</t>
+  </si>
+  <si>
+    <t>Hit the generated link</t>
+  </si>
+  <si>
+    <t>system will open the survey form</t>
+  </si>
+  <si>
+    <t>Fill in the survey form and click at "submit" button</t>
+  </si>
+  <si>
+    <t>system will save that response in database</t>
+  </si>
+  <si>
+    <t>Scope of AlphaVersion Sprint#3</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>total droupout</t>
+  </si>
+  <si>
+    <t>unique droupout</t>
+  </si>
+  <si>
+    <t>last filled field</t>
+  </si>
+  <si>
+    <t>total time spent</t>
+  </si>
+  <si>
+    <t>form complete</t>
+  </si>
+  <si>
+    <t>TS1</t>
+  </si>
+  <si>
+    <t>User hits the url 1 time (does not fill , and does not refresh the url)</t>
+  </si>
+  <si>
+    <t>"total dropout" will turn to 1</t>
+  </si>
+  <si>
+    <t>"Unique dropout" will turn to 1</t>
+  </si>
+  <si>
+    <t>"Null" value will be stored in DB</t>
+  </si>
+  <si>
+    <t>total time of the form in open state at browser (whether active or not)</t>
+  </si>
+  <si>
+    <t>incase of not successful submission 0</t>
+  </si>
+  <si>
+    <t>TS2</t>
+  </si>
+  <si>
+    <t>User hits the url 1 time and successfully submits in first attempt</t>
+  </si>
+  <si>
+    <t>"total dropout" will be "0"</t>
+  </si>
+  <si>
+    <t>"Unique dropout" will be "0"</t>
+  </si>
+  <si>
+    <t>the id of last filled field will be stored in DB</t>
+  </si>
+  <si>
+    <t>will turn to 1 incase of successful submission</t>
+  </si>
+  <si>
+    <t>TS3</t>
+  </si>
+  <si>
+    <t>User hits the URL again which has already been submitted once</t>
+  </si>
+  <si>
+    <t>TS4</t>
+  </si>
+  <si>
+    <t>User hits the url many times without filling any field and without submiting it</t>
+  </si>
+  <si>
+    <t>"total dropout" will increase 1 count per hit</t>
+  </si>
+  <si>
+    <t>TS5</t>
+  </si>
+  <si>
+    <t>User hits the url many times, fills some of the fields and dropout without submiting it</t>
+  </si>
+  <si>
+    <t>"total dropout" will increase 1 count per dropout</t>
+  </si>
+  <si>
+    <t>TS6</t>
+  </si>
+  <si>
+    <t>User hits the url many times, fills some of the fields and dropout and sometimes dropout without filling any field</t>
+  </si>
+  <si>
+    <t>"total dropout" will increase 1 count each time</t>
+  </si>
+  <si>
+    <t>the id of last filled field will be stored in DB (or "Null" if user droppedout last time without filling any field)</t>
+  </si>
+  <si>
+    <t>TS7</t>
+  </si>
+  <si>
+    <t>User hits the URL , In first try user fills the fields and click on submit , but system show error on some invalid data or mandatory field unfilled. Now,user again fills the survey and submit successfully</t>
+  </si>
+  <si>
+    <t>"total dropout" will not change because page will not refresh on error , and will submit next time</t>
+  </si>
+  <si>
+    <t>"unique dropout" will not change because page will not refresh and will submit next time</t>
+  </si>
+  <si>
+    <t>TS8</t>
+  </si>
+  <si>
+    <t>User hits the URL many times and atlast submit it successfully</t>
+  </si>
+  <si>
+    <t>counter will increase at each dropout , but not on submission</t>
+  </si>
+  <si>
+    <t>will turn to 1 at first dropout</t>
+  </si>
+  <si>
+    <t>the id of last filled field at the last dropout will be stored in DB</t>
+  </si>
+  <si>
+    <t>will turn to 1 on successful submission</t>
+  </si>
+  <si>
+    <t>TS9</t>
+  </si>
+  <si>
+    <t>User keeps the URL open on different browsers</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>TS10</t>
+  </si>
+  <si>
+    <t>Fid A with Tid B will have a new record in DB</t>
+  </si>
+  <si>
+    <t>TS11</t>
+  </si>
+  <si>
+    <t>Fid A with Tid C will have a new record in DB</t>
+  </si>
+  <si>
+    <t>TS12</t>
+  </si>
+  <si>
+    <t>Fid C with Tid B will have a new record in DB</t>
+  </si>
+  <si>
+    <t>TS13</t>
+  </si>
+  <si>
+    <t>Fid C with Tid C will have a new record in DB</t>
+  </si>
+  <si>
+    <t>TS14</t>
+  </si>
+  <si>
+    <t>"Completion rate" is the total no. of responses on a survey submitted successfully</t>
+  </si>
+  <si>
+    <t>TS15</t>
+  </si>
+  <si>
+    <t>"Dropout rate" is the total no. of unique dropouts from a particular survey</t>
+  </si>
+  <si>
+    <t>TS16</t>
+  </si>
+  <si>
+    <t>"Open rate" is the total of "Completion rate" and "Dropout rate"</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>Click at "Enable A/B testing" on the dashboard</t>
+  </si>
+  <si>
+    <t>it will open a popup with three dropdowns, and one upload button</t>
+  </si>
+  <si>
+    <t>Select Form A from 1st dropdown and same form A from 2nd dropdown</t>
+  </si>
+  <si>
+    <t>it will show error because of the same form selection in both dropdowns</t>
+  </si>
+  <si>
+    <t>Select Form A from 1st dropdown and another form B from 2nd dropdown</t>
+  </si>
+  <si>
+    <t>it will show both selected forms in both dropdowns</t>
+  </si>
+  <si>
+    <t>Select the A/B test duration from 3rd dropdown and click at "submit" button</t>
+  </si>
+  <si>
+    <t>it will enable the A/B testing on selected forms and will show those selected forms on separate portion on dashboard</t>
+  </si>
+  <si>
+    <t>Randomly open the enabled form URLs and submit input randomly as recipient</t>
+  </si>
+  <si>
+    <t>Analytics will be calculated as per the "Sprint 3 Analytics Scenarios" sheet</t>
+  </si>
+  <si>
+    <t>Hit the cron URL when selected duration get completed</t>
+  </si>
+  <si>
+    <t>it will calculate for winner form , make that winner the default and AB testing will be finished</t>
+  </si>
+  <si>
+    <t>The winning form will be decided on the formula ( open_rate * 0.3 + completion_rate * 0.7)</t>
+  </si>
+  <si>
+    <t>the form with greater result value will be the winner</t>
+  </si>
+  <si>
+    <t>User clicks on "Disable AB testing" on dashboard (while there is an enable AB testing)</t>
+  </si>
+  <si>
+    <t>this will prompt the user for the confirmation</t>
+  </si>
+  <si>
+    <t>Click at "Yes" button on confirmation popup</t>
+  </si>
+  <si>
+    <t>it will disable the AB testing which is in progress</t>
+  </si>
+  <si>
+    <t>Click at "No" button on confirmation popup</t>
+  </si>
+  <si>
+    <t>it will keep executing the AB testing and will close the popup without any action</t>
+  </si>
+  <si>
+    <t>This is the V1.3 of SFF scenarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +795,75 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13.2"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF38761D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF990000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF6AA84F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +885,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -349,10 +962,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -390,8 +1004,52 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -669,34 +1327,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="54.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
     <col min="4" max="4" width="63.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="72.75" thickBot="1">
+    <row r="1" spans="1:7" ht="22.5" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="54.75" thickBot="1">
+      <c r="C1" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" ht="33" customHeight="1" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -713,23 +1376,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="6"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="25.5" customHeight="1" thickBot="1">
-      <c r="A4" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" ht="16.5" thickBot="1">
+    <row r="4" spans="1:7" ht="25.5" customHeight="1" thickBot="1"/>
+    <row r="5" spans="1:7" ht="16.5" thickBot="1">
       <c r="A5" s="3"/>
       <c r="B5" s="7" t="s">
         <v>6</v>
@@ -744,7 +1399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="31.5" thickBot="1">
+    <row r="6" spans="1:7" ht="31.5" thickBot="1">
       <c r="A6" s="3"/>
       <c r="B6" s="7" t="s">
         <v>10</v>
@@ -759,7 +1414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.5" thickBot="1">
+    <row r="7" spans="1:7" ht="31.5" thickBot="1">
       <c r="A7" s="3"/>
       <c r="B7" s="7" t="s">
         <v>13</v>
@@ -774,7 +1429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="31.5" thickBot="1">
+    <row r="8" spans="1:7" ht="31.5" thickBot="1">
       <c r="A8" s="3"/>
       <c r="B8" s="7" t="s">
         <v>14</v>
@@ -789,7 +1444,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="31.5" thickBot="1">
+    <row r="9" spans="1:7" ht="31.5" thickBot="1">
       <c r="A9" s="3"/>
       <c r="B9" s="7" t="s">
         <v>15</v>
@@ -802,14 +1457,14 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="16.5" thickBot="1">
+    <row r="11" spans="1:7" ht="16.5" thickBot="1">
       <c r="A11" s="3"/>
       <c r="B11" s="7" t="s">
         <v>16</v>
@@ -824,7 +1479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.5" thickBot="1">
+    <row r="12" spans="1:7" ht="16.5" thickBot="1">
       <c r="A12" s="3"/>
       <c r="B12" s="7" t="s">
         <v>18</v>
@@ -839,7 +1494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16.5" thickBot="1">
+    <row r="13" spans="1:7" ht="16.5" thickBot="1">
       <c r="A13" s="3"/>
       <c r="B13" s="7" t="s">
         <v>20</v>
@@ -854,7 +1509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16.5" thickBot="1">
+    <row r="14" spans="1:7" ht="16.5" thickBot="1">
       <c r="A14" s="3"/>
       <c r="B14" s="7" t="s">
         <v>22</v>
@@ -869,7 +1524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16.5" thickBot="1">
+    <row r="15" spans="1:7" ht="16.5" thickBot="1">
       <c r="A15" s="3"/>
       <c r="B15" s="7" t="s">
         <v>24</v>
@@ -884,7 +1539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1228,9 +1883,1316 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="C1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="54.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:5" ht="18.75" thickBot="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="36.75" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.5" thickBot="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.5" thickBot="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" thickBot="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="27" thickBot="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="27" thickBot="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A15" s="3"/>
+      <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="31.5" thickBot="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="27" thickBot="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A19" s="3"/>
+      <c r="B19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A21" s="3"/>
+      <c r="B21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="31.5" thickBot="1">
+      <c r="A22" s="3"/>
+      <c r="B22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="31.5" thickBot="1">
+      <c r="A23" s="3"/>
+      <c r="B23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A24" s="3"/>
+      <c r="B24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="31.5" thickBot="1">
+      <c r="A25" s="3"/>
+      <c r="B25" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" ht="31.5" thickBot="1">
+      <c r="A26" s="3"/>
+      <c r="B26" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" ht="52.5" thickBot="1">
+      <c r="A28" s="3"/>
+      <c r="B28" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" ht="27" thickBot="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" ht="76.5" thickBot="1">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="6"/>
+      <c r="D30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" ht="27" thickBot="1">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="D31" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" ht="27" thickBot="1">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" ht="27" thickBot="1">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" ht="27" thickBot="1">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" ht="27" thickBot="1">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A40" s="3"/>
+      <c r="B40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" ht="27" thickBot="1">
+      <c r="A41" s="3"/>
+      <c r="B41" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="6"/>
+      <c r="D41" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" ht="46.5" thickBot="1">
+      <c r="A42" s="3"/>
+      <c r="B42" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="6"/>
+      <c r="D42" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" ht="16.5" thickBot="1">
+      <c r="A44" s="3"/>
+      <c r="B44" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" ht="27" thickBot="1">
+      <c r="A45" s="3"/>
+      <c r="B45" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" ht="27" thickBot="1">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A47" s="3"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E49" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:13" ht="36.75" thickBot="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" ht="18.75" thickBot="1">
+      <c r="A3" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" ht="57.75" customHeight="1" thickBot="1">
+      <c r="A5" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="56.25" customHeight="1" thickBot="1">
+      <c r="A6" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="39.75" thickBot="1">
+      <c r="A7" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="24"/>
+    </row>
+    <row r="8" spans="1:13" ht="43.5" customHeight="1" thickBot="1">
+      <c r="A8" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="78" thickBot="1">
+      <c r="A9" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="78" thickBot="1">
+      <c r="A10" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="90.75" thickBot="1">
+      <c r="A11" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="46.5" customHeight="1" thickBot="1">
+      <c r="A12" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K12" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="27" thickBot="1">
+      <c r="A13" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+    </row>
+    <row r="14" spans="1:13" ht="27" thickBot="1">
+      <c r="A14" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="24"/>
+    </row>
+    <row r="15" spans="1:13" ht="27" thickBot="1">
+      <c r="A15" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="24"/>
+    </row>
+    <row r="16" spans="1:13" ht="27" thickBot="1">
+      <c r="A16" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="24"/>
+    </row>
+    <row r="17" spans="1:13" ht="27" thickBot="1">
+      <c r="A17" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="24"/>
+    </row>
+    <row r="18" spans="1:13" ht="39.75" thickBot="1">
+      <c r="A18" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="24"/>
+    </row>
+    <row r="19" spans="1:13" ht="39.75" thickBot="1">
+      <c r="A19" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="24"/>
+    </row>
+    <row r="20" spans="1:13" ht="39.75" thickBot="1">
+      <c r="A20" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="D19:M19"/>
+    <mergeCell ref="D20:M20"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="D14:M14"/>
+    <mergeCell ref="D15:M15"/>
+    <mergeCell ref="D16:M16"/>
+    <mergeCell ref="D17:M17"/>
+    <mergeCell ref="D18:M18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="55.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="56.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" thickBot="1">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A3" s="25">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="27" thickBot="1">
+      <c r="A4" s="25">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="27" thickBot="1">
+      <c r="A5" s="25">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="27" thickBot="1">
+      <c r="A6" s="25">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A7" s="25">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="27" thickBot="1">
+      <c r="A8" s="25">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="27" thickBot="1">
+      <c r="A9" s="25">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="27" thickBot="1">
+      <c r="A10" s="25">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A11" s="25">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="27" thickBot="1">
+      <c r="A12" s="25">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D7" r:id="rId1" location="gid=251281939" display="https://docs.google.com/spreadsheets/d/1NWwUrfpS74Pa3JJwfruoKLae0plsHm0031aSj4jrlHs/edit - gid=251281939"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
this is the update in scenarios of SFF (V1.4)
</commit_message>
<xml_diff>
--- a/SFF_testscenarios.xlsx
+++ b/SFF_testscenarios.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Prototype1" sheetId="1" r:id="rId1"/>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="169">
   <si>
     <t>Scope of Prototype 1</t>
   </si>
@@ -536,9 +536,6 @@
     <t>TS1</t>
   </si>
   <si>
-    <t>User hits the url 1 time (does not fill , and does not refresh the url)</t>
-  </si>
-  <si>
     <t>"total dropout" will turn to 1</t>
   </si>
   <si>
@@ -557,9 +554,6 @@
     <t>TS2</t>
   </si>
   <si>
-    <t>User hits the url 1 time and successfully submits in first attempt</t>
-  </si>
-  <si>
     <t>"total dropout" will be "0"</t>
   </si>
   <si>
@@ -650,27 +644,15 @@
     <t>TS10</t>
   </si>
   <si>
-    <t>Fid A with Tid B will have a new record in DB</t>
-  </si>
-  <si>
     <t>TS11</t>
   </si>
   <si>
-    <t>Fid A with Tid C will have a new record in DB</t>
-  </si>
-  <si>
     <t>TS12</t>
   </si>
   <si>
-    <t>Fid C with Tid B will have a new record in DB</t>
-  </si>
-  <si>
     <t>TS13</t>
   </si>
   <si>
-    <t>Fid C with Tid C will have a new record in DB</t>
-  </si>
-  <si>
     <t>TS14</t>
   </si>
   <si>
@@ -755,14 +737,38 @@
     <t>it will keep executing the AB testing and will close the popup without any action</t>
   </si>
   <si>
-    <t>This is the V1.3 of SFF scenarios</t>
+    <t>User hits the url 1 time (do not fill , and do not refresh the url)</t>
+  </si>
+  <si>
+    <t>User hits the url 1 time and successfully submit in first attempt</t>
+  </si>
+  <si>
+    <t>Cid A , Tid A , Fid A will have a new record in DB</t>
+  </si>
+  <si>
+    <t>Cid A , Tid A , Fid B is not possible (because tid should be unique for user)</t>
+  </si>
+  <si>
+    <t>Cid A , Tid B , Fid A will have a new record in DB</t>
+  </si>
+  <si>
+    <t>Cid A , Tid B , Fid B is NOT possible (because tid should be unique for user)</t>
+  </si>
+  <si>
+    <t>Cid B , Tid A , Fid A will have a new record (Tid is user specific)</t>
+  </si>
+  <si>
+    <t>TS17</t>
+  </si>
+  <si>
+    <t>This is the V1.4 of SFF scenarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,8 +868,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -897,6 +909,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -966,7 +984,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -995,15 +1013,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1029,6 +1038,24 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1038,13 +1065,34 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1330,9 +1378,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1351,13 +1399,13 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
+      <c r="C1" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="33" customHeight="1" thickBot="1">
       <c r="A2" s="4" t="s">
@@ -1911,7 +1959,7 @@
     <row r="1" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:5" ht="18.75" thickBot="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="3"/>
@@ -2436,11 +2484,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2457,7 +2505,7 @@
     <row r="1" spans="1:13" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:13" ht="36.75" thickBot="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>85</v>
       </c>
       <c r="C2" s="3"/>
@@ -2473,13 +2521,13 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="18.75" thickBot="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="5" t="s">
         <v>87</v>
       </c>
@@ -2504,7 +2552,7 @@
       <c r="K3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="13" t="s">
         <v>91</v>
       </c>
       <c r="M3" s="5" t="s">
@@ -2527,305 +2575,305 @@
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="57.75" customHeight="1" thickBot="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>93</v>
+      <c r="B5" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I5" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="K5" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="56.25" customHeight="1" thickBot="1">
+      <c r="A6" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="M5" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A6" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>100</v>
+      <c r="B6" s="15" t="s">
+        <v>161</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="I6" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="M6" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="45" customHeight="1" thickBot="1">
+      <c r="A7" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="3" t="s">
+      <c r="B7" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="M6" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="39.75" thickBot="1">
-      <c r="A7" s="17" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="27"/>
+    </row>
+    <row r="8" spans="1:13" ht="43.5" customHeight="1" thickBot="1">
+      <c r="A8" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B8" s="15" t="s">
         <v>106</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="24"/>
-    </row>
-    <row r="8" spans="1:13" ht="43.5" customHeight="1" thickBot="1">
-      <c r="A8" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>108</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="39.75" thickBot="1">
+      <c r="A9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>109</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M8" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="78" thickBot="1">
-      <c r="A9" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>111</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="59.25" customHeight="1" thickBot="1">
+      <c r="A10" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>112</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M9" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="78" thickBot="1">
-      <c r="A10" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>114</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="90.75" thickBot="1">
+      <c r="A11" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="B11" s="15" t="s">
         <v>116</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K10" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="M10" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="90.75" thickBot="1">
-      <c r="A11" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>118</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="46.5" customHeight="1" thickBot="1">
+      <c r="A12" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="B12" s="15" t="s">
         <v>120</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="M11" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A12" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>122</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="I12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="21" t="s">
+      <c r="M12" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="27" thickBot="1">
+      <c r="A13" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="I12" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="3" t="s">
+      <c r="B13" s="15" t="s">
         <v>126</v>
-      </c>
-      <c r="M12" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="27" thickBot="1">
-      <c r="A13" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>128</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2835,172 +2883,185 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:13" ht="27" thickBot="1">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:13" ht="30.75" customHeight="1" thickBot="1">
+      <c r="A14" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="30"/>
+    </row>
+    <row r="15" spans="1:13" ht="39.75" thickBot="1">
+      <c r="A15" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="33"/>
+    </row>
+    <row r="16" spans="1:13" ht="27" thickBot="1">
+      <c r="A16" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B16" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="33"/>
+    </row>
+    <row r="17" spans="1:13" ht="42.75" customHeight="1" thickBot="1">
+      <c r="A17" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="24"/>
-    </row>
-    <row r="15" spans="1:13" ht="27" thickBot="1">
-      <c r="A15" s="17" t="s">
+      <c r="B17" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="33"/>
+    </row>
+    <row r="18" spans="1:13" ht="42.75" customHeight="1" thickBot="1">
+      <c r="A18" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B18" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="36"/>
+    </row>
+    <row r="19" spans="1:13" ht="39.75" thickBot="1">
+      <c r="A19" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="24"/>
-    </row>
-    <row r="16" spans="1:13" ht="27" thickBot="1">
-      <c r="A16" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B16" s="18" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="27"/>
+    </row>
+    <row r="20" spans="1:13" ht="39.75" thickBot="1">
+      <c r="A20" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="24"/>
-    </row>
-    <row r="17" spans="1:13" ht="27" thickBot="1">
-      <c r="A17" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="B17" s="18" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
+    </row>
+    <row r="21" spans="1:13" ht="39.75" thickBot="1">
+      <c r="A21" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="24"/>
-    </row>
-    <row r="18" spans="1:13" ht="39.75" thickBot="1">
-      <c r="A18" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="24"/>
-    </row>
-    <row r="19" spans="1:13" ht="39.75" thickBot="1">
-      <c r="A19" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="24"/>
-    </row>
-    <row r="20" spans="1:13" ht="39.75" thickBot="1">
-      <c r="A20" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="24"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="D19:M19"/>
+  <mergeCells count="9">
     <mergeCell ref="D20:M20"/>
+    <mergeCell ref="D21:M21"/>
     <mergeCell ref="D7:M7"/>
     <mergeCell ref="D14:M14"/>
     <mergeCell ref="D15:M15"/>
     <mergeCell ref="D16:M16"/>
     <mergeCell ref="D17:M17"/>
+    <mergeCell ref="D19:M19"/>
     <mergeCell ref="D18:M18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3008,7 +3069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
@@ -3028,10 +3089,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
@@ -3039,152 +3100,152 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A3" s="25">
+      <c r="A3" s="19">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="27" thickBot="1">
-      <c r="A4" s="25">
+      <c r="A4" s="19">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E4" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="27" thickBot="1">
-      <c r="A5" s="25">
+      <c r="A5" s="19">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E5" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="27" thickBot="1">
-      <c r="A6" s="25">
+      <c r="A6" s="19">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A7" s="25">
+      <c r="A7" s="19">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="26" t="s">
+      <c r="D7" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="27" thickBot="1">
-      <c r="A8" s="25">
+      <c r="A8" s="19">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E8" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="27" thickBot="1">
-      <c r="A9" s="25">
+      <c r="A9" s="19">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E9" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="27" thickBot="1">
-      <c r="A10" s="25">
+      <c r="A10" s="19">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A11" s="25">
+      <c r="A11" s="19">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E11" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="27" thickBot="1">
-      <c r="A12" s="25">
+      <c r="A12" s="19">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E12" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>